<commit_message>
Fix Lebar Kolom Tabel
</commit_message>
<xml_diff>
--- a/PangkalanData/public/Template/Template Pesuluh.xlsx
+++ b/PangkalanData/public/Template/Template Pesuluh.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>TEMPLATE IMPORT DATA PESULUH</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Tingkat</t>
-  </si>
-  <si>
-    <t>Kuda</t>
   </si>
   <si>
     <t>Tanda (*) Data Wajib Diisi!</t>
@@ -87,11 +84,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -115,6 +112,29 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -122,16 +142,48 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -145,9 +197,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -155,17 +220,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -176,60 +241,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -237,23 +249,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -304,25 +301,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,55 +457,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -394,97 +475,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -574,15 +571,6 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -602,6 +590,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -620,15 +617,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -675,153 +663,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -834,7 +831,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1211,7 +1208,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -1220,9 +1217,9 @@
     <col min="2" max="2" width="1.55555555555556" style="2" customWidth="1"/>
     <col min="3" max="3" width="5.44444444444444" style="3" customWidth="1"/>
     <col min="4" max="5" width="16.7777777777778" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.4444444444444" style="4" customWidth="1"/>
     <col min="7" max="7" width="16.7777777777778" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5555555555556" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.8888888888889" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.3333333333333" style="1" customWidth="1"/>
     <col min="11" max="13" width="9" style="1"/>
     <col min="14" max="14" width="9.55555555555556" style="1" customWidth="1"/>
@@ -1265,21 +1262,15 @@
       <c r="G2" s="9"/>
       <c r="H2" s="11"/>
     </row>
-    <row r="3" s="1" customFormat="1" ht="15" customHeight="1" spans="1:8">
+    <row r="3" s="1" customFormat="1" ht="15" customHeight="1" spans="1:6">
       <c r="A3" s="9"/>
       <c r="B3" s="2"/>
       <c r="C3" s="12"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="17" customHeight="1" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
@@ -1290,12 +1281,12 @@
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" ht="15.15" spans="1:1">
@@ -1303,12 +1294,12 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" ht="15.15" spans="1:1">
@@ -1316,12 +1307,12 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" ht="15.15" spans="1:1">
@@ -1334,37 +1325,37 @@
     </row>
     <row r="16" ht="15.15" spans="1:1">
       <c r="A16" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1385,8 +1376,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Masukkan Salah" error="Harus Memilih dari Daftar" sqref="H3:H1048576">
       <formula1>$A$17:$A$22</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Masukkan Salah" error="Harus Memilih dari Daftar" sqref="H1:H2"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Masukkan salah" error="Harus sesuai format H/B/T&#10;" sqref="F1:F2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Masukkan Salah" error="Harus Memilih dari Daftar" sqref="H1:H2"/>
     <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Masukkan salah" error="Harus sesuai format H/B/T&#10;" sqref="F3:F1048576">
       <formula1>36892</formula1>
     </dataValidation>

</xml_diff>